<commit_message>
added options and monte carlo
</commit_message>
<xml_diff>
--- a/pca/pca.xlsx
+++ b/pca/pca.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="14310" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="240" windowWidth="27795" windowHeight="14250" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="_ironspread_data_" sheetId="4" state="veryHidden" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1541" uniqueCount="1037">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1628" uniqueCount="1038">
   <si>
     <t>Tickers</t>
   </si>
@@ -3132,6 +3132,9 @@
   </si>
   <si>
     <t>Cutoff:</t>
+  </si>
+  <si>
+    <t>Components:</t>
   </si>
 </sst>
 </file>
@@ -3498,7 +3501,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3556,19 +3559,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <pane ySplit="3000" topLeftCell="A45" activePane="bottomLeft"/>
+      <selection activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="Q52" sqref="Q52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="6.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -3576,7 +3581,7 @@
         <v>14</v>
       </c>
       <c r="B1">
-        <v>100</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -3592,7 +3597,7 @@
         <v>1033</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>1036</v>
@@ -3606,18 +3611,1278 @@
         <v>0</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
+      <c r="D4" s="1" t="s">
+        <v>1037</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="F4" s="3">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="G4" s="3">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="H4" s="3">
+        <v>3.1E-2</v>
+      </c>
+      <c r="I4" s="3">
+        <v>2.3E-2</v>
+      </c>
+      <c r="J4" s="3">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="K4" s="3">
+        <v>1.4E-2</v>
+      </c>
       <c r="L4" s="3"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5">
+        <v>-0.104</v>
+      </c>
+      <c r="F5">
+        <v>-0.377</v>
+      </c>
+      <c r="G5">
+        <v>-0.109</v>
+      </c>
+      <c r="H5">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="I5">
+        <v>-7.8E-2</v>
+      </c>
+      <c r="J5">
+        <v>-0.19900000000000001</v>
+      </c>
+      <c r="K5">
+        <v>0.156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E6">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="F6">
+        <v>2.7E-2</v>
+      </c>
+      <c r="G6">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="H6">
+        <v>-0.187</v>
+      </c>
+      <c r="I6">
+        <v>-0.26</v>
+      </c>
+      <c r="J6">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="K6">
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7">
+        <v>0.13</v>
+      </c>
+      <c r="F7">
+        <v>-0.30399999999999999</v>
+      </c>
+      <c r="G7">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+      <c r="H7">
+        <v>0.157</v>
+      </c>
+      <c r="I7">
+        <v>-1E-3</v>
+      </c>
+      <c r="J7">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="K7">
+        <v>0.129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="F8">
+        <v>0.108</v>
+      </c>
+      <c r="G8">
+        <v>-6.3E-2</v>
+      </c>
+      <c r="H8">
+        <v>0.221</v>
+      </c>
+      <c r="I8">
+        <v>-7.0000000000000001E-3</v>
+      </c>
+      <c r="J8">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="K8">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D9" t="s">
+        <v>191</v>
+      </c>
+      <c r="E9">
+        <v>0.152</v>
+      </c>
+      <c r="F9">
+        <v>-1.7999999999999999E-2</v>
+      </c>
+      <c r="G9">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="H9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I9">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="J9">
+        <v>-5.8999999999999997E-2</v>
+      </c>
+      <c r="K9">
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D10" t="s">
+        <v>193</v>
+      </c>
+      <c r="E10">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="F10">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="G10">
+        <v>-0.106</v>
+      </c>
+      <c r="H10">
+        <v>0.13</v>
+      </c>
+      <c r="I10">
+        <v>-5.2999999999999999E-2</v>
+      </c>
+      <c r="J10">
+        <v>-0.17399999999999999</v>
+      </c>
+      <c r="K10">
+        <v>-2.4E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D11" t="s">
+        <v>225</v>
+      </c>
+      <c r="E11">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="F11">
+        <v>-0.316</v>
+      </c>
+      <c r="G11">
+        <v>0.01</v>
+      </c>
+      <c r="H11">
+        <v>-0.307</v>
+      </c>
+      <c r="I11">
+        <v>6.3E-2</v>
+      </c>
+      <c r="J11">
+        <v>-0.57799999999999996</v>
+      </c>
+      <c r="K11">
+        <v>-0.11799999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D12" t="s">
+        <v>227</v>
+      </c>
+      <c r="E12">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>-3.2000000000000001E-2</v>
+      </c>
+      <c r="H12">
+        <v>-3.3000000000000002E-2</v>
+      </c>
+      <c r="I12">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="J12">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="K12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>271</v>
+      </c>
+      <c r="D13" t="s">
+        <v>271</v>
+      </c>
+      <c r="E13">
+        <v>0.157</v>
+      </c>
+      <c r="F13">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="G13">
+        <v>-9.8000000000000004E-2</v>
+      </c>
+      <c r="H13">
+        <v>-6.7000000000000004E-2</v>
+      </c>
+      <c r="I13">
+        <v>-2.1999999999999999E-2</v>
+      </c>
+      <c r="J13">
+        <v>0.311</v>
+      </c>
+      <c r="K13">
+        <v>-6.5000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>273</v>
+      </c>
+      <c r="D14" t="s">
+        <v>273</v>
+      </c>
+      <c r="E14">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="F14">
+        <v>-0.27100000000000002</v>
+      </c>
+      <c r="G14">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+      <c r="H14">
+        <v>-0.39</v>
+      </c>
+      <c r="I14">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="J14">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="K14">
+        <v>-2.7E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>311</v>
+      </c>
+      <c r="D15" t="s">
+        <v>311</v>
+      </c>
+      <c r="E15">
+        <v>0.159</v>
+      </c>
+      <c r="F15">
+        <v>-0.113</v>
+      </c>
+      <c r="G15">
+        <v>1.4E-2</v>
+      </c>
+      <c r="H15">
+        <v>0.188</v>
+      </c>
+      <c r="I15">
+        <v>-0.19600000000000001</v>
+      </c>
+      <c r="J15">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="K15">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>315</v>
+      </c>
+      <c r="D16" t="s">
+        <v>315</v>
+      </c>
+      <c r="E16">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="F16">
+        <v>-0.20300000000000001</v>
+      </c>
+      <c r="G16">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="H16">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="I16">
+        <v>-0.19900000000000001</v>
+      </c>
+      <c r="J16">
+        <v>0.219</v>
+      </c>
+      <c r="K16">
+        <v>-0.183</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>319</v>
+      </c>
+      <c r="D17" t="s">
+        <v>319</v>
+      </c>
+      <c r="E17">
+        <v>0.17</v>
+      </c>
+      <c r="F17">
+        <v>0.124</v>
+      </c>
+      <c r="G17">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="H17">
+        <v>2E-3</v>
+      </c>
+      <c r="I17">
+        <v>-6.4000000000000001E-2</v>
+      </c>
+      <c r="J17">
+        <v>-7.0000000000000001E-3</v>
+      </c>
+      <c r="K17">
+        <v>-9.7000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>367</v>
+      </c>
+      <c r="D18" t="s">
+        <v>367</v>
+      </c>
+      <c r="E18">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="F18">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="G18">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="H18">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="I18">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="J18">
+        <v>-0.104</v>
+      </c>
+      <c r="K18">
+        <v>5.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>371</v>
+      </c>
+      <c r="D19" t="s">
+        <v>371</v>
+      </c>
+      <c r="E19">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="F19">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="G19">
+        <v>-0.17</v>
+      </c>
+      <c r="H19">
+        <v>-4.2000000000000003E-2</v>
+      </c>
+      <c r="I19">
+        <v>-9.1999999999999998E-2</v>
+      </c>
+      <c r="J19">
+        <v>3.1E-2</v>
+      </c>
+      <c r="K19">
+        <v>-9.0999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>389</v>
+      </c>
+      <c r="D20" t="s">
+        <v>389</v>
+      </c>
+      <c r="E20">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="F20">
+        <v>-5.3999999999999999E-2</v>
+      </c>
+      <c r="G20">
+        <v>-0.03</v>
+      </c>
+      <c r="H20">
+        <v>-2E-3</v>
+      </c>
+      <c r="I20">
+        <v>1E-3</v>
+      </c>
+      <c r="J20">
+        <v>-1.2E-2</v>
+      </c>
+      <c r="K20">
+        <v>3.2000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>421</v>
+      </c>
+      <c r="D21" t="s">
+        <v>421</v>
+      </c>
+      <c r="E21">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="F21">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="G21">
+        <v>-0.13500000000000001</v>
+      </c>
+      <c r="H21">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="I21">
+        <v>-3.5000000000000003E-2</v>
+      </c>
+      <c r="J21">
+        <v>-0.215</v>
+      </c>
+      <c r="K21">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>460</v>
+      </c>
+      <c r="D22" t="s">
+        <v>460</v>
+      </c>
+      <c r="E22">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="F22">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="G22">
+        <v>-0.121</v>
+      </c>
+      <c r="H22">
+        <v>9.4E-2</v>
+      </c>
+      <c r="I22">
+        <v>-1.4999999999999999E-2</v>
+      </c>
+      <c r="J22">
+        <v>-8.6999999999999994E-2</v>
+      </c>
+      <c r="K22">
+        <v>-1.6E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>478</v>
+      </c>
+      <c r="D23" t="s">
+        <v>478</v>
+      </c>
+      <c r="E23">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="F23">
+        <v>-4.8000000000000001E-2</v>
+      </c>
+      <c r="G23">
+        <v>-8.5000000000000006E-2</v>
+      </c>
+      <c r="H23">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="I23">
+        <v>-0.27600000000000002</v>
+      </c>
+      <c r="J23">
+        <v>-0.13700000000000001</v>
+      </c>
+      <c r="K23">
+        <v>-2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>480</v>
+      </c>
+      <c r="D24" t="s">
+        <v>480</v>
+      </c>
+      <c r="E24">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="F24">
+        <v>0.02</v>
+      </c>
+      <c r="G24">
+        <v>-9.2999999999999999E-2</v>
+      </c>
+      <c r="H24">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="I24">
+        <v>-8.1000000000000003E-2</v>
+      </c>
+      <c r="J24">
+        <v>-0.111</v>
+      </c>
+      <c r="K24">
+        <v>3.1E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>552</v>
+      </c>
+      <c r="D25" t="s">
+        <v>552</v>
+      </c>
+      <c r="E25">
+        <v>0.155</v>
+      </c>
+      <c r="F25">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="G25">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="H25">
+        <v>-2.5999999999999999E-2</v>
+      </c>
+      <c r="I25">
+        <v>-0.14799999999999999</v>
+      </c>
+      <c r="J25">
+        <v>-0.128</v>
+      </c>
+      <c r="K25">
+        <v>7.0999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>602</v>
+      </c>
+      <c r="D26" t="s">
+        <v>602</v>
+      </c>
+      <c r="E26">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="F26">
+        <v>-3.6999999999999998E-2</v>
+      </c>
+      <c r="G26">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="H26">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="I26">
+        <v>1.2E-2</v>
+      </c>
+      <c r="J26">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="K26">
+        <v>-4.7E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>604</v>
+      </c>
+      <c r="D27" t="s">
+        <v>604</v>
+      </c>
+      <c r="E27">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="F27">
+        <v>2.3E-2</v>
+      </c>
+      <c r="G27">
+        <v>-0.04</v>
+      </c>
+      <c r="H27">
+        <v>-2.1999999999999999E-2</v>
+      </c>
+      <c r="I27">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="J27">
+        <v>-2.1999999999999999E-2</v>
+      </c>
+      <c r="K27">
+        <v>8.3000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>657</v>
+      </c>
+      <c r="D28" t="s">
+        <v>657</v>
+      </c>
+      <c r="E28">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="F28">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="G28">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="H28">
+        <v>1.2E-2</v>
+      </c>
+      <c r="I28">
+        <v>0.129</v>
+      </c>
+      <c r="J28">
+        <v>-5.2999999999999999E-2</v>
+      </c>
+      <c r="K28">
+        <v>0.25600000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>661</v>
+      </c>
+      <c r="D29" t="s">
+        <v>661</v>
+      </c>
+      <c r="E29">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="F29">
+        <v>-0.192</v>
+      </c>
+      <c r="G29">
+        <v>-0.13600000000000001</v>
+      </c>
+      <c r="H29">
+        <v>-2.4E-2</v>
+      </c>
+      <c r="I29">
+        <v>0.125</v>
+      </c>
+      <c r="J29">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="K29">
+        <v>-0.08</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>665</v>
+      </c>
+      <c r="D30" t="s">
+        <v>665</v>
+      </c>
+      <c r="E30">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="F30">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="G30">
+        <v>-0.10299999999999999</v>
+      </c>
+      <c r="H30">
+        <v>-2.4E-2</v>
+      </c>
+      <c r="I30">
+        <v>-6.2E-2</v>
+      </c>
+      <c r="J30">
+        <v>-0.16700000000000001</v>
+      </c>
+      <c r="K30">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>673</v>
+      </c>
+      <c r="D31" t="s">
+        <v>673</v>
+      </c>
+      <c r="E31">
+        <v>0.161</v>
+      </c>
+      <c r="F31">
+        <v>-2.9000000000000001E-2</v>
+      </c>
+      <c r="G31">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="H31">
+        <v>-0.19</v>
+      </c>
+      <c r="I31">
+        <v>-3.5000000000000003E-2</v>
+      </c>
+      <c r="J31">
+        <v>0.218</v>
+      </c>
+      <c r="K31">
+        <v>5.7000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>685</v>
+      </c>
+      <c r="D32" t="s">
+        <v>685</v>
+      </c>
+      <c r="E32">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="F32">
+        <v>0.08</v>
+      </c>
+      <c r="G32">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="H32">
+        <v>-1.7000000000000001E-2</v>
+      </c>
+      <c r="I32">
+        <v>-2.3E-2</v>
+      </c>
+      <c r="J32">
+        <v>-3.4000000000000002E-2</v>
+      </c>
+      <c r="K32">
+        <v>4.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>687</v>
+      </c>
+      <c r="D33" t="s">
+        <v>687</v>
+      </c>
+      <c r="E33">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="F33">
+        <v>-6.3E-2</v>
+      </c>
+      <c r="G33">
+        <v>4.7E-2</v>
+      </c>
+      <c r="H33">
+        <v>-3.9E-2</v>
+      </c>
+      <c r="I33">
+        <v>-0.1</v>
+      </c>
+      <c r="J33">
+        <v>-1.9E-2</v>
+      </c>
+      <c r="K33">
+        <v>0.13700000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>709</v>
+      </c>
+      <c r="D34" t="s">
+        <v>709</v>
+      </c>
+      <c r="E34">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="F34">
+        <v>-0.10199999999999999</v>
+      </c>
+      <c r="G34">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H34">
+        <v>-5.0999999999999997E-2</v>
+      </c>
+      <c r="I34">
+        <v>-0.122</v>
+      </c>
+      <c r="J34">
+        <v>-0.10299999999999999</v>
+      </c>
+      <c r="K34">
+        <v>0.14299999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>729</v>
+      </c>
+      <c r="D35" t="s">
+        <v>729</v>
+      </c>
+      <c r="E35">
+        <v>-3.3000000000000002E-2</v>
+      </c>
+      <c r="F35">
+        <v>-0.47699999999999998</v>
+      </c>
+      <c r="G35">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="H35">
+        <v>-0.13700000000000001</v>
+      </c>
+      <c r="I35">
+        <v>-0.154</v>
+      </c>
+      <c r="J35">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="K35">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>749</v>
+      </c>
+      <c r="D36" t="s">
+        <v>749</v>
+      </c>
+      <c r="E36">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="F36">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="G36">
+        <v>-0.16800000000000001</v>
+      </c>
+      <c r="H36">
+        <v>-1.0999999999999999E-2</v>
+      </c>
+      <c r="I36">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="J36">
+        <v>-6.2E-2</v>
+      </c>
+      <c r="K36">
+        <v>-0.13500000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>753</v>
+      </c>
+      <c r="D37" t="s">
+        <v>753</v>
+      </c>
+      <c r="E37">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="F37">
+        <v>-3.7999999999999999E-2</v>
+      </c>
+      <c r="G37">
+        <v>-0.16</v>
+      </c>
+      <c r="H37">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="I37">
+        <v>-8.8999999999999996E-2</v>
+      </c>
+      <c r="J37">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="K37">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>797</v>
+      </c>
+      <c r="D38" t="s">
+        <v>797</v>
+      </c>
+      <c r="E38">
+        <v>0.155</v>
+      </c>
+      <c r="F38">
+        <v>-0.111</v>
+      </c>
+      <c r="G38">
+        <v>-0.104</v>
+      </c>
+      <c r="H38">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="I38">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="J38">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="K38">
+        <v>-0.20200000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>819</v>
+      </c>
+      <c r="D39" t="s">
+        <v>819</v>
+      </c>
+      <c r="E39">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="F39">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="G39">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="H39">
+        <v>-0.13100000000000001</v>
+      </c>
+      <c r="I39">
+        <v>-7.2999999999999995E-2</v>
+      </c>
+      <c r="J39">
+        <v>-8.5000000000000006E-2</v>
+      </c>
+      <c r="K39">
+        <v>0.16200000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>833</v>
+      </c>
+      <c r="D40" t="s">
+        <v>833</v>
+      </c>
+      <c r="E40">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="F40">
+        <v>0.05</v>
+      </c>
+      <c r="G40">
+        <v>-6.3E-2</v>
+      </c>
+      <c r="H40">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="I40">
+        <v>-0.112</v>
+      </c>
+      <c r="J40">
+        <v>-5.8000000000000003E-2</v>
+      </c>
+      <c r="K40">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>861</v>
+      </c>
+      <c r="D41" t="s">
+        <v>861</v>
+      </c>
+      <c r="E41">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="F41">
+        <v>-3.9E-2</v>
+      </c>
+      <c r="G41">
+        <v>0.39300000000000002</v>
+      </c>
+      <c r="H41">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="I41">
+        <v>0.311</v>
+      </c>
+      <c r="J41">
+        <v>-4.1000000000000002E-2</v>
+      </c>
+      <c r="K41">
+        <v>0.24399999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>863</v>
+      </c>
+      <c r="D42" t="s">
+        <v>863</v>
+      </c>
+      <c r="E42">
+        <v>0.13</v>
+      </c>
+      <c r="F42">
+        <v>0.108</v>
+      </c>
+      <c r="G42">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="H42">
+        <v>-2.5999999999999999E-2</v>
+      </c>
+      <c r="I42">
+        <v>-1.4E-2</v>
+      </c>
+      <c r="J42">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="K42">
+        <v>0.14099999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>883</v>
+      </c>
+      <c r="D43" t="s">
+        <v>883</v>
+      </c>
+      <c r="E43">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="F43">
+        <v>-0.123</v>
+      </c>
+      <c r="G43">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="H43">
+        <v>-3.3000000000000002E-2</v>
+      </c>
+      <c r="I43">
+        <v>-5.1999999999999998E-2</v>
+      </c>
+      <c r="J43">
+        <v>-0.14499999999999999</v>
+      </c>
+      <c r="K43">
+        <v>-0.71199999999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>905</v>
+      </c>
+      <c r="D44" t="s">
+        <v>905</v>
+      </c>
+      <c r="E44">
+        <v>0.152</v>
+      </c>
+      <c r="F44">
+        <v>0.02</v>
+      </c>
+      <c r="G44">
+        <v>-0.23300000000000001</v>
+      </c>
+      <c r="H44">
+        <v>-0.158</v>
+      </c>
+      <c r="I44">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="J44">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="K44">
+        <v>-7.6999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>955</v>
+      </c>
+      <c r="D45" t="s">
+        <v>955</v>
+      </c>
+      <c r="E45">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="F45">
+        <v>0.05</v>
+      </c>
+      <c r="G45">
+        <v>-0.10199999999999999</v>
+      </c>
+      <c r="H45">
+        <v>-0.02</v>
+      </c>
+      <c r="I45">
+        <v>0.22800000000000001</v>
+      </c>
+      <c r="J45">
+        <v>-3.2000000000000001E-2</v>
+      </c>
+      <c r="K45">
+        <v>-7.3999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>1001</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1001</v>
+      </c>
+      <c r="E46">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="F46">
+        <v>0.113</v>
+      </c>
+      <c r="G46">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H46">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="I46">
+        <v>-0.17899999999999999</v>
+      </c>
+      <c r="J46">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="K46">
+        <v>-0.122</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>1007</v>
+      </c>
+      <c r="D47" t="s">
+        <v>1007</v>
+      </c>
+      <c r="E47">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F47">
+        <v>-0.26300000000000001</v>
+      </c>
+      <c r="G47">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="H47">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="I47">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="J47">
+        <v>-7.1999999999999995E-2</v>
+      </c>
+      <c r="K47">
+        <v>-4.2999999999999997E-2</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>